<commit_message>
Added ViolationService.java to find wrong inputs. Refactored Controller Structure
</commit_message>
<xml_diff>
--- a/doc/views/WebViews.xlsx
+++ b/doc/views/WebViews.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="71">
   <si>
     <t>View</t>
   </si>
@@ -856,7 +856,7 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1006,7 +1006,9 @@
       <c r="E7" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G7" s="27"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1025,7 +1027,9 @@
       <c r="E8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G8" s="27"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Finished the last open tasks.
- Search Series and Users
- Close Requests
- Add Comments to Episodes

Updated WebViews.xlsx
</commit_message>
<xml_diff>
--- a/doc/views/WebViews.xlsx
+++ b/doc/views/WebViews.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="71">
   <si>
     <t>View</t>
   </si>
@@ -183,15 +183,9 @@
     <t>Change Username</t>
   </si>
   <si>
-    <t>currentUser/username</t>
-  </si>
-  <si>
     <t>Change Password</t>
   </si>
   <si>
-    <t>currentUser/password</t>
-  </si>
-  <si>
     <t>Import Movies</t>
   </si>
   <si>
@@ -232,6 +226,12 @@
   </si>
   <si>
     <t>movie, serie</t>
+  </si>
+  <si>
+    <t>user/[id]/password</t>
+  </si>
+  <si>
+    <t>user/[id]/name</t>
   </si>
 </sst>
 </file>
@@ -856,7 +856,7 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -887,10 +887,10 @@
         <v>48</v>
       </c>
       <c r="F1" s="25" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G1" s="25" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -915,7 +915,7 @@
         <v>7</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>13</v>
@@ -935,7 +935,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>15</v>
@@ -953,10 +953,10 @@
         <v>43</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>15</v>
@@ -974,10 +974,10 @@
         <v>43</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>60</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>15</v>
@@ -995,10 +995,10 @@
         <v>7</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>63</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>15</v>
@@ -1016,10 +1016,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>15</v>
@@ -1205,7 +1205,9 @@
         <v>15</v>
       </c>
       <c r="E18" s="23"/>
-      <c r="F18" s="27"/>
+      <c r="F18" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G18" s="27"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1213,7 +1215,7 @@
         <v>44</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>10</v>
@@ -1230,14 +1232,16 @@
         <v>44</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="23"/>
-      <c r="F20" s="27"/>
+      <c r="F20" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G20" s="27"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1267,7 +1271,7 @@
         <v>53</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>15</v>
@@ -1275,7 +1279,9 @@
       <c r="E22" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="27"/>
+      <c r="F22" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G22" s="27"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1283,16 +1289,18 @@
         <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="23"/>
-      <c r="F23" s="27"/>
+      <c r="F23" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G23" s="27"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1332,7 +1340,9 @@
       <c r="E25" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F25" s="27"/>
+      <c r="F25" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G25" s="27"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1372,7 +1382,9 @@
       <c r="E27" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="27"/>
+      <c r="F27" s="27" t="s">
+        <v>15</v>
+      </c>
       <c r="G27" s="27"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1450,7 +1462,9 @@
       <c r="E31" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="28"/>
+      <c r="F31" s="28" t="s">
+        <v>15</v>
+      </c>
       <c r="G31" s="28"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added the file ApiDocumentation.xlsx with the total and complete API Documentation Small changes to the error response code to match responseApi.html
</commit_message>
<xml_diff>
--- a/doc/views/WebViews.xlsx
+++ b/doc/views/WebViews.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="74">
   <si>
     <t>View</t>
   </si>
@@ -232,6 +232,15 @@
   </si>
   <si>
     <t>user/[id]/name</t>
+  </si>
+  <si>
+    <t>Error Page</t>
+  </si>
+  <si>
+    <t>{all movies}</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -853,10 +862,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G56"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -932,31 +941,27 @@
         <v>0</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>2</v>
+        <v>71</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>15</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D4" s="7"/>
+      <c r="E4" s="23"/>
       <c r="F4" s="27" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="G4" s="27"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>15</v>
@@ -974,10 +979,10 @@
         <v>43</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>15</v>
@@ -992,13 +997,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>7</v>
+        <v>43</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>15</v>
@@ -1016,10 +1021,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>15</v>
@@ -1034,16 +1039,20 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>3</v>
+        <v>60</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="23"/>
+        <v>62</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>15</v>
+      </c>
       <c r="F9" s="27" t="s">
         <v>15</v>
       </c>
@@ -1054,10 +1063,10 @@
         <v>0</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="23"/>
@@ -1071,14 +1080,12 @@
         <v>0</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>15</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D11" s="7"/>
       <c r="E11" s="23"/>
       <c r="F11" s="27" t="s">
         <v>15</v>
@@ -1087,13 +1094,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>15</v>
@@ -1106,15 +1113,17 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="7"/>
+        <v>49</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="E13" s="23"/>
       <c r="F13" s="27" t="s">
         <v>15</v>
@@ -1126,10 +1135,10 @@
         <v>0</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="23"/>
@@ -1143,10 +1152,10 @@
         <v>0</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="23"/>
@@ -1160,10 +1169,10 @@
         <v>0</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="23"/>
@@ -1177,14 +1186,12 @@
         <v>0</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>15</v>
-      </c>
+        <v>25</v>
+      </c>
+      <c r="D17" s="7"/>
       <c r="E17" s="23"/>
       <c r="F17" s="27" t="s">
         <v>15</v>
@@ -1193,13 +1200,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>52</v>
+        <v>26</v>
       </c>
       <c r="D18" s="7" t="s">
         <v>15</v>
@@ -1212,15 +1219,17 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="7"/>
+        <v>52</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>15</v>
+      </c>
       <c r="E19" s="23"/>
       <c r="F19" s="27" t="s">
         <v>15</v>
@@ -1232,10 +1241,10 @@
         <v>44</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>9</v>
+        <v>66</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="23"/>
@@ -1246,17 +1255,15 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>28</v>
+        <v>67</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>15</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D21" s="7"/>
       <c r="E21" s="23"/>
       <c r="F21" s="27" t="s">
         <v>15</v>
@@ -1265,20 +1272,18 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>70</v>
+        <v>29</v>
       </c>
       <c r="D22" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E22" s="23" t="s">
-        <v>15</v>
-      </c>
+      <c r="E22" s="23"/>
       <c r="F22" s="27" t="s">
         <v>15</v>
       </c>
@@ -1289,15 +1294,17 @@
         <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D23" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="23"/>
+      <c r="E23" s="23" t="s">
+        <v>15</v>
+      </c>
       <c r="F23" s="27" t="s">
         <v>15</v>
       </c>
@@ -1305,20 +1312,18 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="D24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="23" t="s">
-        <v>15</v>
-      </c>
+      <c r="E24" s="23"/>
       <c r="F24" s="27" t="s">
         <v>15</v>
       </c>
@@ -1326,13 +1331,13 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>44</v>
+        <v>0</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D25" s="7" t="s">
         <v>15</v>
@@ -1347,13 +1352,13 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>15</v>
@@ -1368,13 +1373,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>43</v>
+        <v>0</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D27" s="7" t="s">
         <v>15</v>
@@ -1389,13 +1394,13 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D28" s="7" t="s">
         <v>15</v>
@@ -1413,15 +1418,17 @@
         <v>0</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D29" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="23"/>
+      <c r="E29" s="23" t="s">
+        <v>15</v>
+      </c>
       <c r="F29" s="27" t="s">
         <v>15</v>
       </c>
@@ -1429,13 +1436,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D30" s="7" t="s">
         <v>15</v>
@@ -1446,30 +1453,45 @@
       </c>
       <c r="G30" s="27"/>
     </row>
-    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="10" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="23"/>
+      <c r="F31" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="27"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B32" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C32" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="E31" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="G31" s="28"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="1"/>
-      <c r="D32" s="3"/>
+      <c r="D32" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F32" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="28"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" s="1"/>
@@ -1535,29 +1557,33 @@
       <c r="C48" s="1"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C49" s="1"/>
       <c r="D49" s="3"/>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D50" s="3"/>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D54" s="3"/>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D55" s="3"/>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated away from API, is now again full application
</commit_message>
<xml_diff>
--- a/doc/views/WebViews.xlsx
+++ b/doc/views/WebViews.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DCF822-61C2-4BF3-9565-8B6F96F17862}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="73">
   <si>
     <t>View</t>
   </si>
@@ -238,15 +239,12 @@
   </si>
   <si>
     <t>{all movies}</t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -861,11 +859,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="C6" sqref="A1:G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,9 +946,7 @@
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="23"/>
-      <c r="F4" s="27" t="s">
-        <v>73</v>
-      </c>
+      <c r="F4" s="27"/>
       <c r="G4" s="27"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>